<commit_message>
Added new grouped datasets.
</commit_message>
<xml_diff>
--- a/data/Database/GroupedDataSets.xlsx
+++ b/data/Database/GroupedDataSets.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="122">
   <si>
     <t xml:space="preserve">experimentId</t>
   </si>
@@ -152,6 +152,240 @@
   </si>
   <si>
     <t xml:space="preserve">NLA_057</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_906</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9 lines versus isogenic controls (Isaacs)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9 line 1 merged</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_047</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9 line 2 merged</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_052</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9 line 3 merged</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_051</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9 line 1 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_032</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9 line 1 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_033</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9 line 1 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9 line 2 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_042</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9 line 2 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_043</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9 line 2 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_044</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9 line 3 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_053</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9 line 3 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_054</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9 line 3 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_055</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_907</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Control lines treated with 92-repeat lentivirus versus 2-repeat control (Isaacs)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(G4C2)92 merged</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_048</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(G4C2)92 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(G4C2)92 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_039</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(G4C2)92 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_038</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_908</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9 lines treated with C9 ASOs versus NT ASOs (Isaacs)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9 line 1 ASO merged</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9 line 3 ASO merged</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_050</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9 line 1 ASO 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_036</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9 line 1 ASO 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_040</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9 line 1 ASO 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_041</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9 line 2 ASO 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_037</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9 line 3 ASO 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_045</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9 line 3 ASO 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_046</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_909</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9 lines treated with FAT-1 or FAT-2 lentiviruses (Isaacs)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9 line 1 FAT-1/2 merged</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_068</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9 line 2 FAT-1/2 merged</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_069</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9 line 3 FAT-1/2 merged</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_070</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9 line 1 FAT-1/2 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_060</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9 line 1 FAT-1/2 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_061</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9 line 1 FAT-1/2 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_064</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9 line 2 FAT-1/2 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_063</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9 line 2 FAT-1/2 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_066</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9 line 3 FAT-1/2 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_059</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9 line 3 FAT-1/2 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_062</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9 line 3 FAT-1/2 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_065</t>
   </si>
 </sst>
 </file>
@@ -166,6 +400,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -265,13 +500,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+      <selection pane="topLeft" activeCell="B51" activeCellId="0" sqref="B51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="73.1"/>
@@ -559,6 +794,496 @@
         <v>43</v>
       </c>
     </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>121</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Fixed mixup in titles.
</commit_message>
<xml_diff>
--- a/data/Database/GroupedDataSets.xlsx
+++ b/data/Database/GroupedDataSets.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="126">
   <si>
     <t xml:space="preserve">experimentId</t>
   </si>
@@ -103,22 +103,34 @@
     <t xml:space="preserve">NLA_903</t>
   </si>
   <si>
+    <t xml:space="preserve">ApoE3 iAstrocytes FBS versus no FBS (Feringa and Koppes-den Hertog)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_904</t>
+  </si>
+  <si>
     <t xml:space="preserve">Control vs reactive (IL1a_TNF_C1q) ApoE3 iAstrocytes (Feringa and Koppes-den Hertog)</t>
   </si>
   <si>
-    <t xml:space="preserve">NLA_014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NLA_021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NLA_004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NLA_008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NLA_904</t>
+    <t xml:space="preserve">NLA_010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_905</t>
   </si>
   <si>
     <t xml:space="preserve">Human brain AD vs control (Feringa and Koppes-den Hertog)</t>
@@ -142,7 +154,7 @@
     <t xml:space="preserve">NLA_029</t>
   </si>
   <si>
-    <t xml:space="preserve">NLA_905</t>
+    <t xml:space="preserve">NLA_906</t>
   </si>
   <si>
     <t xml:space="preserve">Human brain FTLD vs control (Isaacs)</t>
@@ -154,7 +166,7 @@
     <t xml:space="preserve">NLA_057</t>
   </si>
   <si>
-    <t xml:space="preserve">NLA_906</t>
+    <t xml:space="preserve">NLA_907</t>
   </si>
   <si>
     <t xml:space="preserve">C9 lines versus isogenic controls (Isaacs)</t>
@@ -232,7 +244,7 @@
     <t xml:space="preserve">NLA_055</t>
   </si>
   <si>
-    <t xml:space="preserve">NLA_907</t>
+    <t xml:space="preserve">NLA_908</t>
   </si>
   <si>
     <t xml:space="preserve">Control lines treated with 92-repeat lentivirus versus 2-repeat control (Isaacs)</t>
@@ -262,7 +274,7 @@
     <t xml:space="preserve">NLA_038</t>
   </si>
   <si>
-    <t xml:space="preserve">NLA_908</t>
+    <t xml:space="preserve">NLA_909</t>
   </si>
   <si>
     <t xml:space="preserve">C9 lines treated with C9 ASOs versus NT ASOs (Isaacs)</t>
@@ -316,7 +328,7 @@
     <t xml:space="preserve">NLA_046</t>
   </si>
   <si>
-    <t xml:space="preserve">NLA_909</t>
+    <t xml:space="preserve">NLA_910</t>
   </si>
   <si>
     <t xml:space="preserve">C9 lines treated with FAT-1 or FAT-2 lentiviruses (Isaacs)</t>
@@ -395,7 +407,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -418,18 +430,31 @@
       <family val="0"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF5CE"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -466,7 +491,11 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -475,12 +504,24 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -492,6 +533,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFF5CE"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -500,788 +601,817 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B51" activeCellId="0" sqref="B51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="73.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="81.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="26.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="1" width="11.56"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+    <row r="5" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+    <row r="6" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+    <row r="7" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+    <row r="12" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
+    <row r="13" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
+    <row r="14" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
+    <row r="15" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="0" t="s">
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="0" t="s">
+    <row r="18" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="B18" s="6" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" s="6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+    <row r="19" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="D19" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="0" t="s">
+    </row>
+    <row r="20" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="B20" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="s">
+      <c r="D20" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="D21" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B22" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D21" s="0" t="s">
+      <c r="C22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="0" t="s">
+    <row r="23" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="B23" s="6" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="D23" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="0" t="s">
+    <row r="24" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D24" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="C25" s="0" t="s">
+    <row r="25" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="D25" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" s="0" t="s">
+    <row r="26" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D26" s="0" t="s">
+      <c r="D26" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27" s="0" t="s">
+    <row r="27" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D27" s="0" t="s">
+      <c r="D27" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28" s="0" t="s">
+    <row r="28" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D28" s="0" t="s">
+      <c r="D28" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="C29" s="0" t="s">
+    <row r="29" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D29" s="0" t="s">
+      <c r="D29" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B30" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="C30" s="0" t="s">
+    <row r="30" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="D30" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B31" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="C31" s="0" t="s">
+    <row r="31" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D31" s="0" t="s">
+      <c r="D31" s="6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="C32" s="0" t="s">
+    <row r="32" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D32" s="0" t="s">
+      <c r="D32" s="6" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+    <row r="33" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="D33" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C33" s="0" t="s">
+    </row>
+    <row r="34" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D33" s="0" t="s">
+      <c r="D34" s="6" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B34" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="C34" s="0" t="s">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D34" s="0" t="s">
+      <c r="B35" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B35" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="C35" s="0" t="s">
+      <c r="C35" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D35" s="0" t="s">
+      <c r="D35" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B36" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="C36" s="0" t="s">
+      <c r="A36" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D36" s="0" t="s">
+      <c r="D36" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="A37" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="D37" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C37" s="0" t="s">
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D37" s="0" t="s">
+      <c r="D38" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="B38" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C38" s="0" t="s">
+    <row r="39" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="D38" s="0" t="s">
+      <c r="B39" s="6" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="B39" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C39" s="0" t="s">
+      <c r="C39" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D39" s="0" t="s">
+      <c r="D39" s="6" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="B40" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C40" s="0" t="s">
+    <row r="40" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C40" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="D40" s="0" t="s">
+      <c r="D40" s="6" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="B41" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C41" s="0" t="s">
+    <row r="41" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D41" s="0" t="s">
+      <c r="D41" s="6" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="B42" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C42" s="0" t="s">
+    <row r="42" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="D42" s="0" t="s">
+      <c r="D42" s="6" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="B43" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C43" s="0" t="s">
+    <row r="43" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C43" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="D43" s="0" t="s">
+      <c r="D43" s="6" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="B44" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C44" s="0" t="s">
+    <row r="44" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C44" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D44" s="0" t="s">
+      <c r="D44" s="6" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+    <row r="45" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C45" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="D45" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C45" s="0" t="s">
+    </row>
+    <row r="46" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C46" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="D45" s="0" t="s">
+      <c r="D46" s="6" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="B46" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="C46" s="0" t="s">
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D46" s="0" t="s">
+      <c r="B47" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="B47" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="C47" s="0" t="s">
+      <c r="C47" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D47" s="0" t="s">
+      <c r="D47" s="1" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="B48" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="C48" s="0" t="s">
+      <c r="A48" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D48" s="0" t="s">
+      <c r="D48" s="1" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="B49" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="C49" s="0" t="s">
+      <c r="A49" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D49" s="0" t="s">
+      <c r="D49" s="1" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="B50" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="C50" s="0" t="s">
+      <c r="A50" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D50" s="0" t="s">
+      <c r="D50" s="1" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="B51" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="C51" s="0" t="s">
+      <c r="A51" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D51" s="0" t="s">
+      <c r="D51" s="1" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="B52" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="C52" s="0" t="s">
+      <c r="A52" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D52" s="0" t="s">
+      <c r="D52" s="1" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="B53" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="C53" s="0" t="s">
+      <c r="A53" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D53" s="0" t="s">
+      <c r="D53" s="1" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="B54" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="C54" s="0" t="s">
+      <c r="A54" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D54" s="0" t="s">
+      <c r="D54" s="1" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="B55" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="C55" s="0" t="s">
+      <c r="A55" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D55" s="0" t="s">
+      <c r="D55" s="1" t="s">
         <v>121</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed grouped experiment NLA_912.
</commit_message>
<xml_diff>
--- a/data/Database/GroupedDataSets.xlsx
+++ b/data/Database/GroupedDataSets.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="155">
   <si>
     <t xml:space="preserve">experimentId</t>
   </si>
@@ -482,6 +482,9 @@
   </si>
   <si>
     <t xml:space="preserve">NLA_089</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_090</t>
   </si>
 </sst>
 </file>
@@ -575,7 +578,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -604,10 +607,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -617,6 +616,22 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF5CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -688,10 +703,10 @@
   <dimension ref="A1:D73"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15:D16"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="89.65"/>
@@ -713,7 +728,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
@@ -727,7 +742,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -797,133 +812,133 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
+    <row r="8" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="s">
+    <row r="9" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="s">
+    <row r="10" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
+    <row r="11" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
+    <row r="12" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="s">
+    <row r="13" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="s">
+    <row r="14" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="s">
+    <row r="15" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="s">
+    <row r="16" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" s="6" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
         <v>36</v>
       </c>
@@ -1718,7 +1733,7 @@
         <v>24</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some subtitles where a bit long, fixed now.
</commit_message>
<xml_diff>
--- a/data/Database/GroupedDataSets.xlsx
+++ b/data/Database/GroupedDataSets.xlsx
@@ -460,13 +460,13 @@
     <t xml:space="preserve">NLA_082</t>
   </si>
   <si>
-    <t xml:space="preserve">Kolf2.1J C156R (hom3) #1 I</t>
+    <t xml:space="preserve">Kolf2.1J C156R #1 I</t>
   </si>
   <si>
     <t xml:space="preserve">NLA_080</t>
   </si>
   <si>
-    <t xml:space="preserve">Kolf2.1J C156R (hom3) #1 II</t>
+    <t xml:space="preserve">Kolf2.1J C156R #1 II</t>
   </si>
   <si>
     <t xml:space="preserve">NLA_084</t>
@@ -616,22 +616,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF5CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -702,11 +686,11 @@
   </sheetPr>
   <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C71" activeCellId="0" sqref="C71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="89.65"/>

</xml_diff>

<commit_message>
Added meta data for Tom.
</commit_message>
<xml_diff>
--- a/data/Database/GroupedDataSets.xlsx
+++ b/data/Database/GroupedDataSets.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="165">
   <si>
     <t xml:space="preserve">experimentId</t>
   </si>
@@ -485,6 +485,36 @@
   </si>
   <si>
     <t xml:space="preserve">NLA_090</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_913</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genotype C22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_092</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genotype C3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_093</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_914</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tom – Age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_094</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_095</t>
   </si>
 </sst>
 </file>
@@ -578,28 +608,36 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -679,1045 +717,1207 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D73"/>
+  <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C71" activeCellId="0" sqref="C71"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A47" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B77" activeCellId="0" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="89.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="89.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="26.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+    <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+    <row r="4" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
+    <row r="5" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+    <row r="6" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+    <row r="7" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
+    <row r="8" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
+    <row r="9" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
+    <row r="10" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
+    <row r="11" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
+    <row r="12" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
+    <row r="13" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
+    <row r="14" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="s">
+    <row r="15" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="s">
+    <row r="16" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" s="6" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="s">
+    <row r="17" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="s">
+    <row r="18" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="s">
+    <row r="19" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="20" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5" t="s">
+    <row r="20" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="6" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="D22" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="D23" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D24" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="D25" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C26" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D26" s="0" t="s">
+      <c r="D26" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="s">
+    <row r="27" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5" t="s">
+    <row r="28" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="29" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5" t="s">
+    <row r="29" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="6" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="C30" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="D30" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C31" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D31" s="0" t="s">
+      <c r="D31" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="5" t="s">
+    <row r="32" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="33" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="5" t="s">
+    <row r="33" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="34" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="5" t="s">
+    <row r="34" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="6" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="35" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="5" t="s">
+    <row r="35" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="6" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="36" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="5" t="s">
+    <row r="36" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="6" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="37" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="5" t="s">
+    <row r="37" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="6" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="38" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="5" t="s">
+    <row r="38" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="39" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="5" t="s">
+    <row r="39" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C39" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="6" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="40" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="5" t="s">
+    <row r="40" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="D40" s="6" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="41" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="5" t="s">
+    <row r="41" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" s="6" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="42" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="5" t="s">
+    <row r="42" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D42" s="6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="43" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="5" t="s">
+    <row r="43" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C43" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="D43" s="6" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="A44" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B44" s="0" t="s">
+      <c r="B44" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C44" s="0" t="s">
+      <c r="C44" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D44" s="0" t="s">
+      <c r="D44" s="1" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="A45" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="B45" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C45" s="0" t="s">
+      <c r="C45" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D45" s="0" t="s">
+      <c r="D45" s="1" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="A46" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B46" s="0" t="s">
+      <c r="B46" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C46" s="0" t="s">
+      <c r="C46" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D46" s="0" t="s">
+      <c r="D46" s="1" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+      <c r="A47" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B47" s="0" t="s">
+      <c r="B47" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C47" s="0" t="s">
+      <c r="C47" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D47" s="0" t="s">
+      <c r="D47" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="48" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="5" t="s">
+    <row r="48" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="C48" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="D48" s="6" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="49" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="5" t="s">
+    <row r="49" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="C49" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="D49" s="6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="50" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="5" t="s">
+    <row r="50" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="C50" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="D50" s="6" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="51" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="5" t="s">
+    <row r="51" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B51" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="C51" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="D51" s="5" t="s">
+      <c r="D51" s="6" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="52" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="5" t="s">
+    <row r="52" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="C52" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="D52" s="5" t="s">
+      <c r="D52" s="6" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="53" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="5" t="s">
+    <row r="53" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B53" s="5" t="s">
+      <c r="B53" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C53" s="5" t="s">
+      <c r="C53" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="D53" s="5" t="s">
+      <c r="D53" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="54" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="5" t="s">
+    <row r="54" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B54" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C54" s="5" t="s">
+      <c r="C54" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="D54" s="5" t="s">
+      <c r="D54" s="6" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="55" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="5" t="s">
+    <row r="55" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B55" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="C55" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="D55" s="5" t="s">
+      <c r="D55" s="6" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+      <c r="A56" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B56" s="0" t="s">
+      <c r="B56" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C56" s="0" t="s">
+      <c r="C56" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D56" s="0" t="s">
+      <c r="D56" s="1" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
+      <c r="A57" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B57" s="0" t="s">
+      <c r="B57" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C57" s="0" t="s">
+      <c r="C57" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D57" s="0" t="s">
+      <c r="D57" s="1" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
+      <c r="A58" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B58" s="0" t="s">
+      <c r="B58" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C58" s="0" t="s">
+      <c r="C58" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D58" s="0" t="s">
+      <c r="D58" s="1" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
+      <c r="A59" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B59" s="0" t="s">
+      <c r="B59" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C59" s="0" t="s">
+      <c r="C59" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D59" s="0" t="s">
+      <c r="D59" s="1" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
+      <c r="A60" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B60" s="0" t="s">
+      <c r="B60" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C60" s="0" t="s">
+      <c r="C60" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D60" s="0" t="s">
+      <c r="D60" s="1" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
+      <c r="A61" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B61" s="0" t="s">
+      <c r="B61" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C61" s="0" t="s">
+      <c r="C61" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="D61" s="0" t="s">
+      <c r="D61" s="1" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
+      <c r="A62" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B62" s="0" t="s">
+      <c r="B62" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C62" s="0" t="s">
+      <c r="C62" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D62" s="0" t="s">
+      <c r="D62" s="1" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
+      <c r="A63" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B63" s="0" t="s">
+      <c r="B63" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C63" s="0" t="s">
+      <c r="C63" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D63" s="0" t="s">
+      <c r="D63" s="1" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
+      <c r="A64" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B64" s="0" t="s">
+      <c r="B64" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C64" s="0" t="s">
+      <c r="C64" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D64" s="0" t="s">
+      <c r="D64" s="1" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
+      <c r="A65" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B65" s="0" t="s">
+      <c r="B65" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C65" s="0" t="s">
+      <c r="C65" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D65" s="0" t="s">
+      <c r="D65" s="1" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+      <c r="A66" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B66" s="0" t="s">
+      <c r="B66" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C66" s="0" t="s">
+      <c r="C66" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D66" s="0" t="s">
+      <c r="D66" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="67" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="5" t="s">
+    <row r="67" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B67" s="5" t="s">
+      <c r="B67" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="C67" s="5" t="s">
+      <c r="C67" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="D67" s="5" t="s">
+      <c r="D67" s="6" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="68" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="5" t="s">
+    <row r="68" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="B68" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="C68" s="5" t="s">
+      <c r="C68" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="D68" s="5" t="s">
+      <c r="D68" s="6" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="69" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="5" t="s">
+    <row r="69" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B69" s="5" t="s">
+      <c r="B69" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="C69" s="5" t="s">
+      <c r="C69" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="D69" s="5" t="s">
+      <c r="D69" s="6" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="70" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="5" t="s">
+    <row r="70" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B70" s="5" t="s">
+      <c r="B70" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="C70" s="5" t="s">
+      <c r="C70" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="D70" s="5" t="s">
+      <c r="D70" s="6" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
+      <c r="A71" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B71" s="0" t="s">
+      <c r="B71" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C71" s="0" t="s">
+      <c r="C71" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D71" s="0" t="s">
+      <c r="D71" s="1" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
+      <c r="A72" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B72" s="0" t="s">
+      <c r="B72" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C72" s="0" t="s">
+      <c r="C72" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D72" s="0" t="s">
+      <c r="D72" s="1" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
+      <c r="A73" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B73" s="0" t="s">
+      <c r="B73" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C73" s="0" t="s">
+      <c r="C73" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D73" s="0" t="s">
+      <c r="D73" s="1" t="s">
         <v>154</v>
+      </c>
+    </row>
+    <row r="74" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="75" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Toms data without TGs.
</commit_message>
<xml_diff>
--- a/data/Database/GroupedDataSets.xlsx
+++ b/data/Database/GroupedDataSets.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="176">
   <si>
     <t xml:space="preserve">experimentId</t>
   </si>
@@ -515,6 +515,103 @@
   </si>
   <si>
     <t xml:space="preserve">NLA_095</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_915</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tom (no TG)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Genotype C22</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (no TG)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_097</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Tom</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (no TG)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Genotype C3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (no TG)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_098</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_916</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Tom – Age</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (no TG)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_099</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_100</t>
   </si>
 </sst>
 </file>
@@ -524,7 +621,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -558,6 +655,11 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -717,124 +819,18 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
-  <a:themeElements>
-    <a:clrScheme name="LibreOffice">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="000000"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="ffffff"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="18a303"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="0369a3"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a33e03"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8e03a3"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="c99c00"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="c9211e"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000ee"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="551a8b"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D77"/>
+  <dimension ref="A1:D81"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A47" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B77" activeCellId="0" sqref="B77"/>
+      <selection pane="topLeft" activeCell="B70" activeCellId="0" sqref="B70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="89.65"/>
@@ -1920,6 +1916,62 @@
         <v>164</v>
       </c>
     </row>
+    <row r="78" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="79" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Expanded on Toms data and fixed some mistakes in the meta data.
</commit_message>
<xml_diff>
--- a/data/Database/GroupedDataSets.xlsx
+++ b/data/Database/GroupedDataSets.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="188">
   <si>
     <t xml:space="preserve">experimentId</t>
   </si>
@@ -514,79 +514,19 @@
     <t xml:space="preserve">NLA_094</t>
   </si>
   <si>
+    <t xml:space="preserve">NLA_096</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_915</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tom – Age (WT)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genotype C22 – WT</t>
+  </si>
+  <si>
     <t xml:space="preserve">NLA_095</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NLA_915</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tom (no TG)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Genotype C22</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (no TG)</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">NLA_097</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Tom</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (no TG)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Genotype C3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (no TG)</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">NLA_098</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NLA_916</t>
   </si>
   <si>
     <r>
@@ -604,14 +544,62 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> (no TG)</t>
+      <t xml:space="preserve"> (WT)</t>
     </r>
   </si>
   <si>
+    <t xml:space="preserve">Genotype C3 – WT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_097</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_916</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tom (no TG)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genotype C22 (no TG)</t>
+  </si>
+  <si>
     <t xml:space="preserve">NLA_099</t>
   </si>
   <si>
+    <t xml:space="preserve">Genotype C3 (no TG)</t>
+  </si>
+  <si>
     <t xml:space="preserve">NLA_100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_917</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tom – Age (no TG)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_918</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tom – Age (no TG) (WT)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genotype C22 – WT (no TG)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genotype C3 – WT (no TG)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_104</t>
   </si>
 </sst>
 </file>
@@ -710,7 +698,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -744,6 +732,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -824,13 +820,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:D85"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A47" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B70" activeCellId="0" sqref="B70"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B47" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D86" activeCellId="0" sqref="D86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="89.65"/>
@@ -1944,32 +1940,88 @@
         <v>171</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="1" t="s">
+    <row r="80" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B80" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="C80" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D80" s="1" t="s">
+      <c r="C80" s="9" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="1" t="s">
+      <c r="D80" s="9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="81" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B81" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="C81" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>175</v>
+      <c r="C81" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="D81" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="82" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="83" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="84" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="B84" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="C84" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="D84" s="9" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="85" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="B85" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="C85" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="D85" s="9" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final datasets for Tom.
</commit_message>
<xml_diff>
--- a/data/Database/GroupedDataSets.xlsx
+++ b/data/Database/GroupedDataSets.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="175">
   <si>
     <t xml:space="preserve">experimentId</t>
   </si>
@@ -490,116 +490,61 @@
     <t xml:space="preserve">NLA_913</t>
   </si>
   <si>
-    <t xml:space="preserve">Tom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Genotype C22</t>
+    <t xml:space="preserve">Longitudinal analysis of lipid changes in the sciatic nerve caused by overexpression of PMP22 in models of CMT1A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_091</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C22 – WT</t>
   </si>
   <si>
     <t xml:space="preserve">NLA_092</t>
   </si>
   <si>
-    <t xml:space="preserve">Genotype C3</t>
+    <t xml:space="preserve">C3</t>
   </si>
   <si>
     <t xml:space="preserve">NLA_093</t>
   </si>
   <si>
+    <t xml:space="preserve">C3 – WT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_094</t>
+  </si>
+  <si>
     <t xml:space="preserve">NLA_914</t>
   </si>
   <si>
-    <t xml:space="preserve">Tom – Age</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NLA_094</t>
+    <t xml:space="preserve">Longitudinal analysis of lipid changes in the sciatic nerve caused by overexpression of PMP22 in models of CMT1A (no TG)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C22 (no TG)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_095</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C22 – WT (no TG)</t>
   </si>
   <si>
     <t xml:space="preserve">NLA_096</t>
   </si>
   <si>
-    <t xml:space="preserve">NLA_915</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tom – Age (WT)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Genotype C22 – WT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NLA_095</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Tom – Age</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (WT)</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Genotype C3 – WT</t>
+    <t xml:space="preserve">C3 (no TG)</t>
   </si>
   <si>
     <t xml:space="preserve">NLA_097</t>
   </si>
   <si>
-    <t xml:space="preserve">NLA_916</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tom (no TG)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Genotype C22 (no TG)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NLA_099</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Genotype C3 (no TG)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NLA_100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NLA_917</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tom – Age (no TG)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NLA_101</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NLA_103</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NLA_918</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tom – Age (no TG) (WT)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Genotype C22 – WT (no TG)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NLA_102</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Genotype C3 – WT (no TG)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NLA_104</t>
+    <t xml:space="preserve">C3 – WT (no TG)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_098</t>
   </si>
 </sst>
 </file>
@@ -609,7 +554,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -643,11 +588,6 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -820,16 +760,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D85"/>
+  <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B47" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D86" activeCellId="0" sqref="D86"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A47" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B81" activeCellId="0" sqref="B81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="89.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="106.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="26.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.57"/>
   </cols>
@@ -1884,144 +1824,88 @@
         <v>160</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="1" t="s">
+    <row r="76" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C76" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="D76" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="C76" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D76" s="1" t="s">
+    </row>
+    <row r="77" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C77" s="6" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D77" s="1" t="s">
+      <c r="D77" s="6" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="78" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="6" t="s">
+    <row r="78" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="B78" s="6" t="s">
+      <c r="B78" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="C78" s="6" t="s">
+      <c r="C78" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="D78" s="6" t="s">
+      <c r="D78" s="9" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="79" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="6" t="s">
+    <row r="79" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="B79" s="6" t="s">
+      <c r="B79" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C79" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="C79" s="6" t="s">
+      <c r="D79" s="9" t="s">
         <v>170</v>
-      </c>
-      <c r="D79" s="6" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="80" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="B80" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C80" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D80" s="9" t="s">
         <v>172</v>
-      </c>
-      <c r="B80" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="C80" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="D80" s="9" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="81" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="9" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="B81" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C81" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="C81" s="9" t="s">
-        <v>176</v>
-      </c>
       <c r="D81" s="9" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="82" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="B82" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="C82" s="6" t="s">
         <v>174</v>
-      </c>
-      <c r="D82" s="6" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="83" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="B83" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="C83" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="D83" s="6" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="84" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="B84" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="C84" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="D84" s="9" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="85" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="B85" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="C85" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="D85" s="9" t="s">
-        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more comparisons for Tom and added missing meta data.
</commit_message>
<xml_diff>
--- a/data/Database/GroupedDataSets.xlsx
+++ b/data/Database/GroupedDataSets.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="218">
   <si>
     <t xml:space="preserve">experimentId</t>
   </si>
@@ -545,6 +545,135 @@
   </si>
   <si>
     <t xml:space="preserve">NLA_098</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_915</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longitudinal analysis of lipid changes in the sciatic nerve caused by overexpression of PMP22 in models of CMT1A (C22 – C3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C22 vs C22 – WT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_099</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C3 vs C3 – WT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_916</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longitudinal analysis of lipid changes in the sciatic nerve caused by overexpression of PMP22 in models of CMT1A (C22 – C3) (no TG)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_917</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longitudinal analysis of lipid changes in the sciatic nerve caused by overexpression of PMP22 in models of CMT1A (C22 age)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 weeks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 weeks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_104</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 weeks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 weeks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_106</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 weeks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_107</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_918</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longitudinal analysis of lipid changes in the sciatic nerve caused by overexpression of PMP22 in models of CMT1A (C22 age) (no TG)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_108</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_109</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_919</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longitudinal analysis of lipid changes in the sciatic nerve caused by overexpression of PMP22 in models of CMT1A (C3 age)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_113</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_114</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_116</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_117</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_920</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longitudinal analysis of lipid changes in the sciatic nerve caused by overexpression of PMP22 in models of CMT1A (C3 age) (no TG)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_118</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_119</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_121</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLA_122</t>
   </si>
 </sst>
 </file>
@@ -638,7 +767,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -676,10 +805,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -760,16 +885,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:D105"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A47" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B81" activeCellId="0" sqref="B81"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A62" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B101" activeCellId="0" sqref="B101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="106.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="110.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="26.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.57"/>
   </cols>
@@ -1852,60 +1977,396 @@
         <v>164</v>
       </c>
     </row>
-    <row r="78" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="9" t="s">
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="B78" s="9" t="s">
+      <c r="B78" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="C78" s="9" t="s">
+      <c r="C78" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="D78" s="9" t="s">
+      <c r="D78" s="4" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="79" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="9" t="s">
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="B79" s="9" t="s">
+      <c r="B79" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="C79" s="9" t="s">
+      <c r="C79" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="D79" s="9" t="s">
+      <c r="D79" s="4" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="80" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="9" t="s">
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="B80" s="9" t="s">
+      <c r="B80" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="C80" s="9" t="s">
+      <c r="C80" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="D80" s="9" t="s">
+      <c r="D80" s="4" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="81" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="9" t="s">
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="B81" s="9" t="s">
+      <c r="B81" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="C81" s="9" t="s">
+      <c r="C81" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="D81" s="9" t="s">
+      <c r="D81" s="4" t="s">
         <v>174</v>
+      </c>
+    </row>
+    <row r="82" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="83" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="86" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D86" s="6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="87" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="D87" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="88" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="B88" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="D88" s="6" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="89" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="C89" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="D89" s="6" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="90" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="C90" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="D90" s="6" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="96" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B96" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="C96" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D96" s="6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="97" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B97" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="C97" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="D97" s="6" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="98" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B98" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="C98" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="D98" s="6" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="99" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B99" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="C99" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="D99" s="6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="100" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B100" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="C100" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="D100" s="6" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D101" s="9" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D102" s="9" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D103" s="9" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D104" s="9" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D105" s="9" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>